<commit_message>
Added ExtractOptimal class Added column size logic Relative testing
</commit_message>
<xml_diff>
--- a/Testing/Risultati/benchmark_results_Levenshtein_10_output.xlsx
+++ b/Testing/Risultati/benchmark_results_Levenshtein_10_output.xlsx
@@ -7,8 +7,7 @@
   </bookViews>
   <sheets>
     <sheet name="Benchmark Data" r:id="rId3" sheetId="1"/>
-    <sheet name="Memory Usage Data" r:id="rId4" sheetId="2"/>
-    <sheet name="Average Memory Usage" r:id="rId6" sheetId="3"/>
+    <sheet name="Average Memory Usage" r:id="rId6" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -1335,12 +1334,32 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="darkGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1355,8 +1374,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -1393,23 +1414,23 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s" s="1">
         <v>7</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
+      <c r="B2" s="1"/>
+      <c r="C2" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="1">
         <v>11</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s" s="1">
         <v>12</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s" s="1">
         <v>13</v>
       </c>
     </row>
@@ -1437,25 +1458,25 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="0">
+      <c r="C4" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="G4" t="s" s="0">
+      <c r="G4" t="s" s="2">
         <v>21</v>
       </c>
     </row>
@@ -2709,25 +2730,25 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="s" s="0">
+      <c r="A60" t="s" s="1">
         <v>139</v>
       </c>
-      <c r="B60" t="s" s="0">
+      <c r="B60" t="s" s="1">
         <v>18</v>
       </c>
-      <c r="C60" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D60" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E60" t="s" s="0">
+      <c r="C60" t="s" s="1">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s" s="1">
+        <v>10</v>
+      </c>
+      <c r="E60" t="s" s="1">
         <v>144</v>
       </c>
-      <c r="F60" t="s" s="0">
+      <c r="F60" t="s" s="1">
         <v>145</v>
       </c>
-      <c r="G60" t="s" s="0">
+      <c r="G60" t="s" s="1">
         <v>21</v>
       </c>
     </row>
@@ -2824,23 +2845,23 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="0">
+      <c r="A65" t="s" s="2">
         <v>154</v>
       </c>
-      <c r="B65" s="0"/>
-      <c r="C65" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D65" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E65" t="s" s="0">
+      <c r="B65" s="2"/>
+      <c r="C65" t="s" s="2">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="E65" t="s" s="2">
         <v>155</v>
       </c>
-      <c r="F65" t="s" s="0">
+      <c r="F65" t="s" s="2">
         <v>156</v>
       </c>
-      <c r="G65" t="s" s="0">
+      <c r="G65" t="s" s="2">
         <v>13</v>
       </c>
     </row>
@@ -3942,1307 +3963,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B161"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="0">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>258</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B13" t="s" s="0">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B14" t="s" s="0">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B15" t="s" s="0">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B16" t="s" s="0">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B17" t="s" s="0">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B18" t="s" s="0">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B19" t="s" s="0">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B20" t="s" s="0">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="0">
-        <v>269</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B22" t="s" s="0">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B23" t="s" s="0">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B24" t="s" s="0">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B25" t="s" s="0">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B26" t="s" s="0">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B27" t="s" s="0">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B28" t="s" s="0">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B29" t="s" s="0">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B30" t="s" s="0">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="0">
-        <v>280</v>
-      </c>
-      <c r="B31" t="s" s="0">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B32" t="s" s="0">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B33" t="s" s="0">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B34" t="s" s="0">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B35" t="s" s="0">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B36" t="s" s="0">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B37" t="s" s="0">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B38" t="s" s="0">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B39" t="s" s="0">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B40" t="s" s="0">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="0">
-        <v>291</v>
-      </c>
-      <c r="B41" t="s" s="0">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B42" t="s" s="0">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B43" t="s" s="0">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B44" t="s" s="0">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B45" t="s" s="0">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B46" t="s" s="0">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B47" t="s" s="0">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B48" t="s" s="0">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B49" t="s" s="0">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B50" t="s" s="0">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="0">
-        <v>302</v>
-      </c>
-      <c r="B51" t="s" s="0">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B52" t="s" s="0">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B53" t="s" s="0">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B54" t="s" s="0">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B55" t="s" s="0">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B56" t="s" s="0">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B57" t="s" s="0">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B58" t="s" s="0">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B59" t="s" s="0">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B60" t="s" s="0">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="0">
-        <v>313</v>
-      </c>
-      <c r="B61" t="s" s="0">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B62" t="s" s="0">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B63" t="s" s="0">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B64" t="s" s="0">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B65" t="s" s="0">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B66" t="s" s="0">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B67" t="s" s="0">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B68" t="s" s="0">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B69" t="s" s="0">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B70" t="s" s="0">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s" s="0">
-        <v>324</v>
-      </c>
-      <c r="B71" t="s" s="0">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B72" t="s" s="0">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B73" t="s" s="0">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B74" t="s" s="0">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B75" t="s" s="0">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B76" t="s" s="0">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B77" t="s" s="0">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B78" t="s" s="0">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B79" t="s" s="0">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B80" t="s" s="0">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="0">
-        <v>335</v>
-      </c>
-      <c r="B81" t="s" s="0">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B82" t="s" s="0">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B83" t="s" s="0">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B84" t="s" s="0">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B85" t="s" s="0">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B86" t="s" s="0">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B87" t="s" s="0">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B88" t="s" s="0">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B89" t="s" s="0">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B90" t="s" s="0">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s" s="0">
-        <v>346</v>
-      </c>
-      <c r="B91" t="s" s="0">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B92" t="s" s="0">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B93" t="s" s="0">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B94" t="s" s="0">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B95" t="s" s="0">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B96" t="s" s="0">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B97" t="s" s="0">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B98" t="s" s="0">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B99" t="s" s="0">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B100" t="s" s="0">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="0">
-        <v>357</v>
-      </c>
-      <c r="B101" t="s" s="0">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B102" t="s" s="0">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B103" t="s" s="0">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B104" t="s" s="0">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B105" t="s" s="0">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B106" t="s" s="0">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B107" t="s" s="0">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B108" t="s" s="0">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B109" t="s" s="0">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B110" t="s" s="0">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s" s="0">
-        <v>368</v>
-      </c>
-      <c r="B111" t="s" s="0">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B112" t="s" s="0">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B113" t="s" s="0">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B114" t="s" s="0">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B115" t="s" s="0">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B116" t="s" s="0">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B117" t="s" s="0">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B118" t="s" s="0">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B119" t="s" s="0">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B120" t="s" s="0">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="121">
-      <c r="A121" t="s" s="0">
-        <v>379</v>
-      </c>
-      <c r="B121" t="s" s="0">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B122" t="s" s="0">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B123" t="s" s="0">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B124" t="s" s="0">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B125" t="s" s="0">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B126" t="s" s="0">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B127" t="s" s="0">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B128" t="s" s="0">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B129" t="s" s="0">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B130" t="s" s="0">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="s" s="0">
-        <v>390</v>
-      </c>
-      <c r="B131" t="s" s="0">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B132" t="s" s="0">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B133" t="s" s="0">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B134" t="s" s="0">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B135" t="s" s="0">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B136" t="s" s="0">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B137" t="s" s="0">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B138" t="s" s="0">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B139" t="s" s="0">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B140" t="s" s="0">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="s" s="0">
-        <v>401</v>
-      </c>
-      <c r="B141" t="s" s="0">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B142" t="s" s="0">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B143" t="s" s="0">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B144" t="s" s="0">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B145" t="s" s="0">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B146" t="s" s="0">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B147" t="s" s="0">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B148" t="s" s="0">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B149" t="s" s="0">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B150" t="s" s="0">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="s" s="0">
-        <v>412</v>
-      </c>
-      <c r="B151" t="s" s="0">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B152" t="s" s="0">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B153" t="s" s="0">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B154" t="s" s="0">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B155" t="s" s="0">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B156" t="s" s="0">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B157" t="s" s="0">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B158" t="s" s="0">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B159" t="s" s="0">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B160" t="s" s="0">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="s" s="0">
-        <v>423</v>
-      </c>
-      <c r="B161" t="s" s="0">
-        <v>433</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B17"/>
   <sheetViews>

</xml_diff>